<commit_message>
cambio de nombre a files
los files tenian nombres incorrectos
</commit_message>
<xml_diff>
--- a/data/descargas_sala_situacional/POSITIVIDAD_20052020.xlsx
+++ b/data/descargas_sala_situacional/POSITIVIDAD_20052020.xlsx
@@ -1,24 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ogti050\Desktop\COVID\20052020\ENVIAR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA_SALA_SITUACIONAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3976B493-7239-48C2-9683-8673017DF9E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3CE43341-5918-46E6-9F33-95D79B323EA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11610" yWindow="240" windowWidth="28800" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{8E98435A-7FD3-469B-8512-3D99A10BA11D}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -153,9 +159,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,11 +474,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B3CA096-4503-4D38-A50D-6736486DEFEA}">
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,13 +515,13 @@
         <v>6</v>
       </c>
       <c r="C2">
-        <v>395239</v>
+        <v>224601</v>
       </c>
       <c r="D2">
-        <v>67060</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0.16969999999999999</v>
+        <v>32339</v>
+      </c>
+      <c r="E2">
+        <v>14.399999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -527,13 +532,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>32554</v>
+        <v>18164</v>
       </c>
       <c r="D3">
-        <v>7381</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0.22670000000000001</v>
+        <v>4245</v>
+      </c>
+      <c r="E3">
+        <v>23.369999999999997</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -544,13 +549,13 @@
         <v>8</v>
       </c>
       <c r="C4">
-        <v>31978</v>
+        <v>15613</v>
       </c>
       <c r="D4">
-        <v>2072</v>
-      </c>
-      <c r="E4" s="1">
-        <v>6.4799999999999996E-2</v>
+        <v>763</v>
+      </c>
+      <c r="E4">
+        <v>4.8899999999999997</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -558,16 +563,16 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C5">
-        <v>23671</v>
+        <v>14165</v>
       </c>
       <c r="D5">
-        <v>2447</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0.10340000000000001</v>
+        <v>3008</v>
+      </c>
+      <c r="E5">
+        <v>21.240000000000002</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -575,16 +580,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C6">
-        <v>22720</v>
+        <v>13599</v>
       </c>
       <c r="D6">
-        <v>5409</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0.23810000000000001</v>
+        <v>1804</v>
+      </c>
+      <c r="E6">
+        <v>13.270000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -592,16 +597,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7">
-        <v>20900</v>
+        <v>12503</v>
       </c>
       <c r="D7">
-        <v>3335</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0.15959999999999999</v>
+        <v>1062</v>
+      </c>
+      <c r="E7">
+        <v>8.49</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -612,13 +617,13 @@
         <v>12</v>
       </c>
       <c r="C8">
-        <v>20292</v>
+        <v>12098</v>
       </c>
       <c r="D8">
-        <v>2354</v>
-      </c>
-      <c r="E8" s="1">
-        <v>0.11600000000000001</v>
+        <v>1159</v>
+      </c>
+      <c r="E8">
+        <v>9.58</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -626,16 +631,16 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C9">
-        <v>16305</v>
+        <v>8389</v>
       </c>
       <c r="D9">
-        <v>1769</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0.1085</v>
+        <v>587</v>
+      </c>
+      <c r="E9">
+        <v>7.0000000000000009</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -643,16 +648,16 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C10">
-        <v>15497</v>
+        <v>7784</v>
       </c>
       <c r="D10">
-        <v>1223</v>
-      </c>
-      <c r="E10" s="1">
-        <v>7.8899999999999998E-2</v>
+        <v>1595</v>
+      </c>
+      <c r="E10">
+        <v>20.49</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -660,16 +665,16 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C11">
-        <v>13586</v>
+        <v>7300</v>
       </c>
       <c r="D11">
-        <v>654</v>
-      </c>
-      <c r="E11" s="1">
-        <v>4.8099999999999997E-2</v>
+        <v>698</v>
+      </c>
+      <c r="E11">
+        <v>9.56</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -677,16 +682,16 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C12">
-        <v>12424</v>
+        <v>6487</v>
       </c>
       <c r="D12">
-        <v>3085</v>
-      </c>
-      <c r="E12" s="1">
-        <v>0.24829999999999999</v>
+        <v>303</v>
+      </c>
+      <c r="E12">
+        <v>4.67</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -694,16 +699,16 @@
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C13">
-        <v>12394</v>
+        <v>6271</v>
       </c>
       <c r="D13">
-        <v>822</v>
-      </c>
-      <c r="E13" s="1">
-        <v>6.6299999999999998E-2</v>
+        <v>322</v>
+      </c>
+      <c r="E13">
+        <v>5.13</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -711,16 +716,16 @@
         <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C14">
-        <v>10347</v>
+        <v>6162</v>
       </c>
       <c r="D14">
-        <v>217</v>
-      </c>
-      <c r="E14" s="1">
-        <v>2.1000000000000001E-2</v>
+        <v>249</v>
+      </c>
+      <c r="E14">
+        <v>4.04</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -728,16 +733,16 @@
         <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C15">
-        <v>10144</v>
+        <v>6153</v>
       </c>
       <c r="D15">
-        <v>451</v>
-      </c>
-      <c r="E15" s="1">
-        <v>4.4499999999999998E-2</v>
+        <v>149</v>
+      </c>
+      <c r="E15">
+        <v>2.42</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -745,16 +750,16 @@
         <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C16">
-        <v>9444</v>
+        <v>5952</v>
       </c>
       <c r="D16">
-        <v>242</v>
-      </c>
-      <c r="E16" s="1">
-        <v>2.5600000000000001E-2</v>
+        <v>144</v>
+      </c>
+      <c r="E16">
+        <v>2.42</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -762,16 +767,16 @@
         <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C17">
-        <v>9296</v>
+        <v>5652</v>
       </c>
       <c r="D17">
-        <v>2371</v>
-      </c>
-      <c r="E17" s="1">
-        <v>0.25509999999999999</v>
+        <v>124</v>
+      </c>
+      <c r="E17">
+        <v>2.19</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -779,16 +784,16 @@
         <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C18">
-        <v>7878</v>
+        <v>5271</v>
       </c>
       <c r="D18">
-        <v>235</v>
-      </c>
-      <c r="E18" s="1">
-        <v>2.98E-2</v>
+        <v>1032</v>
+      </c>
+      <c r="E18">
+        <v>19.580000000000002</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -796,16 +801,16 @@
         <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C19">
-        <v>7705</v>
+        <v>4782</v>
       </c>
       <c r="D19">
-        <v>259</v>
-      </c>
-      <c r="E19" s="1">
-        <v>3.3599999999999998E-2</v>
+        <v>255</v>
+      </c>
+      <c r="E19">
+        <v>5.33</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -813,16 +818,16 @@
         <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C20">
-        <v>7599</v>
+        <v>4421</v>
       </c>
       <c r="D20">
-        <v>539</v>
-      </c>
-      <c r="E20" s="1">
-        <v>7.0900000000000005E-2</v>
+        <v>142</v>
+      </c>
+      <c r="E20">
+        <v>3.2099999999999995</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -833,13 +838,13 @@
         <v>25</v>
       </c>
       <c r="C21">
-        <v>6763</v>
+        <v>3927</v>
       </c>
       <c r="D21">
-        <v>702</v>
-      </c>
-      <c r="E21" s="1">
-        <v>0.1038</v>
+        <v>378</v>
+      </c>
+      <c r="E21">
+        <v>9.629999999999999</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -850,13 +855,13 @@
         <v>26</v>
       </c>
       <c r="C22">
-        <v>6267</v>
+        <v>3701</v>
       </c>
       <c r="D22">
-        <v>260</v>
-      </c>
-      <c r="E22" s="1">
-        <v>4.1500000000000002E-2</v>
+        <v>203</v>
+      </c>
+      <c r="E22">
+        <v>5.4899999999999993</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -864,16 +869,16 @@
         <v>5</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C23">
-        <v>6025</v>
+        <v>3694</v>
       </c>
       <c r="D23">
-        <v>231</v>
-      </c>
-      <c r="E23" s="1">
-        <v>3.8300000000000001E-2</v>
+        <v>111</v>
+      </c>
+      <c r="E23">
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -884,13 +889,13 @@
         <v>28</v>
       </c>
       <c r="C24">
-        <v>5947</v>
+        <v>3576</v>
       </c>
       <c r="D24">
-        <v>440</v>
-      </c>
-      <c r="E24" s="1">
-        <v>7.3999999999999996E-2</v>
+        <v>181</v>
+      </c>
+      <c r="E24">
+        <v>5.0599999999999996</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -898,16 +903,16 @@
         <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C25">
-        <v>5489</v>
+        <v>3203</v>
       </c>
       <c r="D25">
-        <v>113</v>
-      </c>
-      <c r="E25" s="1">
-        <v>2.06E-2</v>
+        <v>170</v>
+      </c>
+      <c r="E25">
+        <v>5.3100000000000005</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -915,16 +920,16 @@
         <v>5</v>
       </c>
       <c r="B26" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C26">
-        <v>4959</v>
+        <v>3111</v>
       </c>
       <c r="D26">
-        <v>349</v>
-      </c>
-      <c r="E26" s="1">
-        <v>7.0400000000000004E-2</v>
+        <v>166</v>
+      </c>
+      <c r="E26">
+        <v>5.34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>